<commit_message>
main2.py is a work in progress
</commit_message>
<xml_diff>
--- a/Input_lecct.xlsx
+++ b/Input_lecct.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fer/PycharmProjects/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B38A80-63B0-9641-A180-6CB32B6DD457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DF10DE-F601-F84A-8AC3-104910DBEFF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27360" yWindow="4300" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{D0582A75-A442-7A41-B2A5-85D1C2251066}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{D0582A75-A442-7A41-B2A5-85D1C2251066}"/>
   </bookViews>
   <sheets>
-    <sheet name="Arcs" sheetId="1" r:id="rId1"/>
-    <sheet name="Commodities" sheetId="2" r:id="rId2"/>
+    <sheet name="Vertex" sheetId="3" r:id="rId1"/>
+    <sheet name="Arcs" sheetId="1" r:id="rId2"/>
+    <sheet name="Commodities" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>i</t>
   </si>
@@ -59,6 +60,9 @@
   </si>
   <si>
     <t>quant</t>
+  </si>
+  <si>
+    <t>vertex</t>
   </si>
 </sst>
 </file>
@@ -409,11 +413,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B49858E9-287D-4940-B877-90D9247CA0E9}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16C6B190-B7FB-004A-909C-CF6F86B57582}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView zoomScale="251" zoomScaleNormal="251" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -532,15 +581,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5607BFC-FA57-3646-8893-93BA788B94F9}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView zoomScale="263" zoomScaleNormal="263" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>